<commit_message>
E170 Engine Model Update
E170 Engine Model Update
</commit_message>
<xml_diff>
--- a/Data/E170.xlsx
+++ b/Data/E170.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="2" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="4" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Vehicle" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="877" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="878" uniqueCount="255">
   <si>
     <t>Wing</t>
   </si>
@@ -776,9 +776,6 @@
     <t xml:space="preserve"> Monday, 09. July 2018 07:05:06 PM</t>
   </si>
   <si>
-    <t xml:space="preserve"> Tuesday, 10. July 2018 09:45:00 PM</t>
-  </si>
-  <si>
     <t>Wednesday, 11. July 2018 08:29:54</t>
   </si>
   <si>
@@ -789,14 +786,24 @@
   </si>
   <si>
     <t>WERED</t>
+  </si>
+  <si>
+    <t>DIFF</t>
+  </si>
+  <si>
+    <t>Tuesday, 17. July 2018 09:24:30 PM</t>
+  </si>
+  <si>
+    <t>Normalizando</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.00000"/>
+    <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -998,7 +1005,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1103,6 +1110,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1559,13 +1568,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1480</c:v>
+                  <c:v>1389</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2202</c:v>
+                  <c:v>2067</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2548</c:v>
+                  <c:v>2389</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1602,11 +1611,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-104697760"/>
-        <c:axId val="-104703744"/>
+        <c:axId val="-1707826112"/>
+        <c:axId val="-1707820128"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-104697760"/>
+        <c:axId val="-1707826112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1696,12 +1705,12 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-104703744"/>
+        <c:crossAx val="-1707820128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-104703744"/>
+        <c:axId val="-1707820128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1805,7 +1814,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-104697760"/>
+        <c:crossAx val="-1707826112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2212,11 +2221,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-104699392"/>
-        <c:axId val="-104700480"/>
+        <c:axId val="-1707819040"/>
+        <c:axId val="-1707820672"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-104699392"/>
+        <c:axId val="-1707819040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.95000000000000007"/>
@@ -2322,12 +2331,12 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-104700480"/>
+        <c:crossAx val="-1707820672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-104700480"/>
+        <c:axId val="-1707820672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2431,7 +2440,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-104699392"/>
+        <c:crossAx val="-1707819040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2838,11 +2847,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-104708640"/>
-        <c:axId val="-104701024"/>
+        <c:axId val="-1707822304"/>
+        <c:axId val="-1707815232"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-104708640"/>
+        <c:axId val="-1707822304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.95000000000000007"/>
@@ -2948,12 +2957,12 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-104701024"/>
+        <c:crossAx val="-1707815232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-104701024"/>
+        <c:axId val="-1707815232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3057,7 +3066,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-104708640"/>
+        <c:crossAx val="-1707822304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3175,6 +3184,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3463,11 +3473,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-104705920"/>
-        <c:axId val="-104707552"/>
+        <c:axId val="-1707816864"/>
+        <c:axId val="-1707817952"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-104705920"/>
+        <c:axId val="-1707816864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.95000000000000007"/>
@@ -3512,6 +3522,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3572,12 +3583,12 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-104707552"/>
+        <c:crossAx val="-1707817952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-104707552"/>
+        <c:axId val="-1707817952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3620,6 +3631,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3680,7 +3692,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-104705920"/>
+        <c:crossAx val="-1707816864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3694,6 +3706,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4085,11 +4098,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-104697216"/>
-        <c:axId val="-104711360"/>
+        <c:axId val="-1707816320"/>
+        <c:axId val="-1707829376"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-104697216"/>
+        <c:axId val="-1707816320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.95000000000000007"/>
@@ -4194,12 +4207,12 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-104711360"/>
+        <c:crossAx val="-1707829376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-104711360"/>
+        <c:axId val="-1707829376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4302,7 +4315,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-104697216"/>
+        <c:crossAx val="-1707816320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7593,7 +7606,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C138"/>
   <sheetViews>
-    <sheetView topLeftCell="A106" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A126" sqref="A126"/>
     </sheetView>
   </sheetViews>
@@ -10197,7 +10210,7 @@
         <v>237</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="F19" s="4" t="s">
         <v>0</v>
@@ -10222,7 +10235,7 @@
         <v>238</v>
       </c>
       <c r="C20" s="33" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="F20" s="3" t="s">
         <v>171</v>
@@ -10486,10 +10499,10 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="34" t="s">
+        <v>248</v>
+      </c>
+      <c r="B46" s="35" t="s">
         <v>249</v>
-      </c>
-      <c r="B46" s="35" t="s">
-        <v>250</v>
       </c>
       <c r="C46" s="36"/>
     </row>
@@ -10500,10 +10513,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E33"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24:E29"/>
+    <sheetView tabSelected="1" topLeftCell="B10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -10713,7 +10726,7 @@
         <v>30164</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="39" t="s">
         <v>180</v>
       </c>
@@ -10723,7 +10736,7 @@
       </c>
       <c r="D17" s="55"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="28" t="s">
         <v>182</v>
       </c>
@@ -10735,7 +10748,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="31" t="s">
         <v>183</v>
       </c>
@@ -10747,7 +10760,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="31" t="s">
         <v>184</v>
       </c>
@@ -10759,7 +10772,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="31" t="s">
         <v>185</v>
       </c>
@@ -10771,7 +10784,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="31" t="s">
         <v>186</v>
       </c>
@@ -10783,7 +10796,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="34" t="s">
         <v>187</v>
       </c>
@@ -10795,7 +10808,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="28" t="s">
         <v>172</v>
       </c>
@@ -10812,7 +10825,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="31" t="s">
         <v>177</v>
       </c>
@@ -10829,7 +10842,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="31">
         <v>0</v>
       </c>
@@ -10842,10 +10855,13 @@
       <c r="D26" s="33">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F26" s="2" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="31">
-        <v>1480</v>
+        <v>1389</v>
       </c>
       <c r="B27" s="32">
         <v>9404</v>
@@ -10856,10 +10872,14 @@
       <c r="D27" s="33">
         <v>37200</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F27" s="58">
+        <f>A27/A12-1</f>
+        <v>3.656716417910455E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="31">
-        <v>2202</v>
+        <v>2067</v>
       </c>
       <c r="B28" s="32">
         <v>7036</v>
@@ -10870,10 +10890,14 @@
       <c r="D28" s="33">
         <v>37200</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F28" s="58">
+        <f t="shared" ref="F28:F29" si="0">A28/A13-1</f>
+        <v>2.3267326732673288E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="31">
-        <v>2548</v>
+        <v>2389</v>
       </c>
       <c r="B29" s="32">
         <v>0</v>
@@ -10884,27 +10908,31 @@
       <c r="D29" s="33">
         <v>30164</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F29" s="58">
+        <f t="shared" si="0"/>
+        <v>2.9741379310344929E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="31"/>
       <c r="B30" s="32"/>
       <c r="C30" s="32"/>
       <c r="D30" s="33"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="34"/>
       <c r="B31" s="35"/>
       <c r="C31" s="35"/>
       <c r="D31" s="36"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>248</v>
+        <v>253</v>
       </c>
     </row>
   </sheetData>
@@ -10922,8 +10950,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AR61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="R17" sqref="R17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -11774,6 +11802,10 @@
       <c r="P11" s="33">
         <f t="shared" si="0"/>
         <v>1.91E-3</v>
+      </c>
+      <c r="Q11" s="59">
+        <f>P11/AR11-1</f>
+        <v>-0.12785388127853881</v>
       </c>
       <c r="AC11" s="31">
         <v>0.6</v>
@@ -16125,8 +16157,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -16643,9 +16675,6 @@
       <c r="D15" s="32" t="s">
         <v>226</v>
       </c>
-      <c r="E15" s="32" t="s">
-        <v>226</v>
-      </c>
       <c r="F15" s="32" t="s">
         <v>226</v>
       </c>
@@ -16662,7 +16691,7 @@
       <c r="F16" s="32"/>
       <c r="G16" s="33"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="31"/>
       <c r="B17" s="32"/>
       <c r="C17" s="32"/>
@@ -16671,29 +16700,23 @@
       <c r="F17" s="32"/>
       <c r="G17" s="33"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="31" t="s">
         <v>130</v>
       </c>
       <c r="B18" s="32"/>
       <c r="C18" s="32"/>
-      <c r="D18" s="32"/>
-      <c r="E18" s="32"/>
-      <c r="F18" s="32"/>
       <c r="G18" s="33"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="31" t="s">
         <v>247</v>
       </c>
       <c r="B19" s="32"/>
       <c r="C19" s="32"/>
-      <c r="D19" s="32"/>
-      <c r="E19" s="32"/>
-      <c r="F19" s="32"/>
       <c r="G19" s="33"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="34"/>
       <c r="B20" s="35"/>
       <c r="C20" s="35"/>
@@ -16702,12 +16725,12 @@
       <c r="F20" s="35"/>
       <c r="G20" s="36"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="28"/>
       <c r="B23" s="29"/>
       <c r="C23" s="29"/>
@@ -16716,7 +16739,7 @@
       <c r="F23" s="29"/>
       <c r="G23" s="30"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="31" t="s">
         <v>246</v>
       </c>
@@ -16739,7 +16762,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="31" t="s">
         <v>223</v>
       </c>
@@ -16762,7 +16785,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="31" t="s">
         <v>223</v>
       </c>
@@ -16785,7 +16808,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="31" t="s">
         <v>227</v>
       </c>
@@ -16808,7 +16831,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="31" t="s">
         <v>228</v>
       </c>
@@ -16831,7 +16854,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="31" t="s">
         <v>229</v>
       </c>
@@ -16853,8 +16876,15 @@
       <c r="G29" s="33">
         <v>0.99</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J29" s="32"/>
+      <c r="K29" s="32">
+        <v>610.45899999999995</v>
+      </c>
+      <c r="L29" s="32">
+        <v>2.164E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="31" t="s">
         <v>230</v>
       </c>
@@ -16876,8 +16906,19 @@
       <c r="G30" s="33">
         <v>0.99</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J30" s="32" t="s">
+        <v>254</v>
+      </c>
+      <c r="K30" s="32">
+        <f>B15*C15/K29</f>
+        <v>2.0375224216532151E-2</v>
+      </c>
+      <c r="L30" s="32">
+        <f>K30/0.02164-1</f>
+        <v>-5.8446200714780461E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="31" t="s">
         <v>231</v>
       </c>
@@ -16900,7 +16941,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="31" t="s">
         <v>232</v>
       </c>

</xml_diff>

<commit_message>
Analise parametrica no payload range diagram
Analise parametrica no payload range diagram
</commit_message>
<xml_diff>
--- a/Data/E170.xlsx
+++ b/Data/E170.xlsx
@@ -17,8 +17,9 @@
     <sheet name="Mission" sheetId="3" r:id="rId3"/>
     <sheet name="Weight_breakdown" sheetId="4" r:id="rId4"/>
     <sheet name="Payload_Range" sheetId="5" r:id="rId5"/>
-    <sheet name="Compr_Drag" sheetId="6" r:id="rId6"/>
-    <sheet name="Parasite_Drag" sheetId="7" r:id="rId7"/>
+    <sheet name="Engine" sheetId="8" r:id="rId6"/>
+    <sheet name="Compr_Drag" sheetId="6" r:id="rId7"/>
+    <sheet name="Parasite_Drag" sheetId="7" r:id="rId8"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="878" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1054" uniqueCount="280">
   <si>
     <t>Wing</t>
   </si>
@@ -791,10 +792,85 @@
     <t>DIFF</t>
   </si>
   <si>
-    <t>Tuesday, 17. July 2018 09:24:30 PM</t>
-  </si>
-  <si>
     <t>Normalizando</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RANGE    </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> nm      </t>
+  </si>
+  <si>
+    <t>ABS</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Tuesday, 24. July 2018 07:30:13 PM</t>
+  </si>
+  <si>
+    <t>Modification</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1.005*BOW</t>
+  </si>
+  <si>
+    <t>oswald 1.</t>
+  </si>
+  <si>
+    <t>Efeitos:</t>
+  </si>
+  <si>
+    <t>Mexer no oswald</t>
+  </si>
+  <si>
+    <t>aparentemente mexe</t>
+  </si>
+  <si>
+    <t>a mesma coisa em cada condicao</t>
+  </si>
+  <si>
+    <t>sendo mais expressivo em 1 e 2</t>
+  </si>
+  <si>
+    <t>Conclusao</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O BOW afeta os pontos </t>
+  </si>
+  <si>
+    <t>1 e 3 sendo mais</t>
+  </si>
+  <si>
+    <t>expressivo em 1</t>
+  </si>
+  <si>
+    <t>Arrasto Induzido</t>
+  </si>
+  <si>
+    <t>Peso</t>
+  </si>
+  <si>
+    <t>motor pressure_ratio fan 1.7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O motor realmente vai </t>
+  </si>
+  <si>
+    <t xml:space="preserve">no sentido de deslocar a </t>
+  </si>
+  <si>
+    <t>curva para a direita se</t>
+  </si>
+  <si>
+    <t>o SFC diminui</t>
+  </si>
+  <si>
+    <t>AR 8.6 p 8.26</t>
+  </si>
+  <si>
+    <t>Mesma conclusao</t>
+  </si>
+  <si>
+    <t>que o oswald</t>
   </si>
 </sst>
 </file>
@@ -1568,13 +1644,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1356</c:v>
+                  <c:v>1381</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2018</c:v>
+                  <c:v>2039</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2323</c:v>
+                  <c:v>2362</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1592,7 +1668,137 @@
                   <c:v>9404</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7036</c:v>
+                  <c:v>7035</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Modified</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:srgbClr val="00B050"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:srgbClr val="00B050"/>
+                    </a:solidFill>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pt-BR"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="1"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Payload_Range!$AB$44:$AB$47</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1427</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2090</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2424</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Payload_Range!$AC$44:$AC$47</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>9404</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9404</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7075</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -1611,11 +1817,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1465078496"/>
-        <c:axId val="1465088288"/>
+        <c:axId val="1793981136"/>
+        <c:axId val="1793987120"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1465078496"/>
+        <c:axId val="1793981136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1705,12 +1911,12 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1465088288"/>
+        <c:crossAx val="1793987120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1465088288"/>
+        <c:axId val="1793987120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1814,7 +2020,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1465078496"/>
+        <c:crossAx val="1793981136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1932,6 +2138,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2220,11 +2427,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1465084480"/>
-        <c:axId val="1465079040"/>
+        <c:axId val="1793986032"/>
+        <c:axId val="1793987664"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1465084480"/>
+        <c:axId val="1793986032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.95000000000000007"/>
@@ -2269,6 +2476,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2329,12 +2537,12 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1465079040"/>
+        <c:crossAx val="1793987664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1465079040"/>
+        <c:axId val="1793987664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2377,6 +2585,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2437,7 +2646,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1465084480"/>
+        <c:crossAx val="1793986032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2451,6 +2660,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2554,6 +2764,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2842,11 +3053,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1465088832"/>
-        <c:axId val="1465082848"/>
+        <c:axId val="1793982224"/>
+        <c:axId val="1793983856"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1465088832"/>
+        <c:axId val="1793982224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.95000000000000007"/>
@@ -2891,6 +3102,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2951,12 +3163,12 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1465082848"/>
+        <c:crossAx val="1793983856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1465082848"/>
+        <c:axId val="1793983856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2999,6 +3211,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3059,7 +3272,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1465088832"/>
+        <c:crossAx val="1793982224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3073,6 +3286,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3464,11 +3678,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1465092640"/>
-        <c:axId val="1465090464"/>
+        <c:axId val="1793973520"/>
+        <c:axId val="1793974064"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1465092640"/>
+        <c:axId val="1793973520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.95000000000000007"/>
@@ -3573,12 +3787,12 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1465090464"/>
+        <c:crossAx val="1793974064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1465090464"/>
+        <c:axId val="1793974064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3681,7 +3895,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1465092640"/>
+        <c:crossAx val="1793973520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4086,11 +4300,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1465092096"/>
-        <c:axId val="1465093184"/>
+        <c:axId val="1793976784"/>
+        <c:axId val="1793662048"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1465092096"/>
+        <c:axId val="1793976784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.95000000000000007"/>
@@ -4195,12 +4409,12 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1465093184"/>
+        <c:crossAx val="1793662048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1465093184"/>
+        <c:axId val="1793662048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4303,7 +4517,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1465092096"/>
+        <c:crossAx val="1793976784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -10501,10 +10715,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:AQ54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24:E29"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -10598,7 +10812,9 @@
       <c r="C7" s="45" t="s">
         <v>124</v>
       </c>
-      <c r="D7" s="33"/>
+      <c r="D7" s="33">
+        <v>1600</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="31" t="s">
@@ -10714,7 +10930,7 @@
         <v>30164</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="39" t="s">
         <v>180</v>
       </c>
@@ -10724,7 +10940,7 @@
       </c>
       <c r="D17" s="57"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="28" t="s">
         <v>182</v>
       </c>
@@ -10735,20 +10951,28 @@
       <c r="D18" s="30" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E18" s="2">
+        <f>C18-B3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="31" t="s">
         <v>183</v>
       </c>
       <c r="B19" s="32"/>
       <c r="C19" s="32">
-        <v>20736</v>
+        <v>20737</v>
       </c>
       <c r="D19" s="33" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E19" s="2">
+        <f>C19-B5</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="31" t="s">
         <v>184</v>
       </c>
@@ -10759,8 +10983,12 @@
       <c r="D20" s="33" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E20" s="2">
+        <f>C20-B4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="31" t="s">
         <v>185</v>
       </c>
@@ -10771,8 +10999,12 @@
       <c r="D21" s="33" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E21" s="2">
+        <f>C21-B7</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="31" t="s">
         <v>186</v>
       </c>
@@ -10783,22 +11015,26 @@
       <c r="D22" s="33" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E22" s="2">
+        <f>C22-B6</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="34" t="s">
         <v>187</v>
       </c>
       <c r="B23" s="35"/>
       <c r="C23" s="35">
-        <v>1750</v>
+        <v>1600</v>
       </c>
       <c r="D23" s="36" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="28" t="s">
-        <v>172</v>
+        <v>254</v>
       </c>
       <c r="B24" s="29" t="s">
         <v>173</v>
@@ -10809,13 +11045,10 @@
       <c r="D24" s="30" t="s">
         <v>175</v>
       </c>
-      <c r="E24" s="2" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="31" t="s">
-        <v>177</v>
+        <v>255</v>
       </c>
       <c r="B25" s="32" t="s">
         <v>178</v>
@@ -10826,11 +11059,8 @@
       <c r="D25" s="33" t="s">
         <v>178</v>
       </c>
-      <c r="E25" s="2" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="31">
         <v>0</v>
       </c>
@@ -10846,31 +11076,38 @@
       <c r="F26" s="2" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G26" s="2" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="31">
-        <v>1356</v>
+        <v>1381</v>
       </c>
       <c r="B27" s="32">
         <v>9404</v>
       </c>
       <c r="C27" s="32">
-        <v>7060</v>
+        <v>7059</v>
       </c>
       <c r="D27" s="33">
         <v>37200</v>
       </c>
       <c r="F27" s="52">
         <f>A27/A12-1</f>
-        <v>1.1940298507462588E-2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+        <v>3.0597014925373145E-2</v>
+      </c>
+      <c r="G27" s="2">
+        <f>A27-A12</f>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="31">
-        <v>2018</v>
+        <v>2039</v>
       </c>
       <c r="B28" s="32">
-        <v>7036</v>
+        <v>7035</v>
       </c>
       <c r="C28" s="32">
         <v>9428</v>
@@ -10880,12 +11117,16 @@
       </c>
       <c r="F28" s="52">
         <f t="shared" ref="F28:F29" si="0">A28/A13-1</f>
-        <v>-9.9009900990099098E-4</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+        <v>9.4059405940594143E-3</v>
+      </c>
+      <c r="G28" s="2">
+        <f t="shared" ref="G28:G29" si="1">A28-A13</f>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="31">
-        <v>2323</v>
+        <v>2362</v>
       </c>
       <c r="B29" s="32">
         <v>0</v>
@@ -10894,40 +11135,1224 @@
         <v>9428</v>
       </c>
       <c r="D29" s="33">
-        <v>30164</v>
+        <v>30165</v>
       </c>
       <c r="F29" s="52">
         <f t="shared" si="0"/>
-        <v>1.293103448275934E-3</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1.8103448275861966E-2</v>
+      </c>
+      <c r="G29" s="2">
+        <f t="shared" si="1"/>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="31"/>
       <c r="B30" s="32"/>
       <c r="C30" s="32"/>
       <c r="D30" s="33"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="34"/>
       <c r="B31" s="35"/>
       <c r="C31" s="35"/>
       <c r="D31" s="36"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>253</v>
+        <v>257</v>
+      </c>
+    </row>
+    <row r="34" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="J34" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="K34" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="M34" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="S34" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="T34" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="V34" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="AB34" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="AC34" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="AK34" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="AL34" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="AN34" s="2" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="35" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="J35" s="39" t="s">
+        <v>180</v>
+      </c>
+      <c r="K35" s="40"/>
+      <c r="L35" s="56" t="s">
+        <v>164</v>
+      </c>
+      <c r="M35" s="57"/>
+      <c r="S35" s="39" t="s">
+        <v>180</v>
+      </c>
+      <c r="T35" s="40"/>
+      <c r="U35" s="56" t="s">
+        <v>164</v>
+      </c>
+      <c r="V35" s="57"/>
+      <c r="AB35" s="39" t="s">
+        <v>180</v>
+      </c>
+      <c r="AC35" s="40"/>
+      <c r="AD35" s="56" t="s">
+        <v>164</v>
+      </c>
+      <c r="AE35" s="57"/>
+      <c r="AG35" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="AK35" s="39" t="s">
+        <v>180</v>
+      </c>
+      <c r="AL35" s="40"/>
+      <c r="AM35" s="56" t="s">
+        <v>164</v>
+      </c>
+      <c r="AN35" s="57"/>
+    </row>
+    <row r="36" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A36" s="39" t="s">
+        <v>180</v>
+      </c>
+      <c r="B36" s="40"/>
+      <c r="C36" s="56" t="s">
+        <v>164</v>
+      </c>
+      <c r="D36" s="57"/>
+      <c r="J36" s="28" t="s">
+        <v>182</v>
+      </c>
+      <c r="K36" s="29"/>
+      <c r="L36" s="29">
+        <v>37200</v>
+      </c>
+      <c r="M36" s="30" t="s">
+        <v>124</v>
+      </c>
+      <c r="O36" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="S36" s="28" t="s">
+        <v>182</v>
+      </c>
+      <c r="T36" s="29"/>
+      <c r="U36" s="29">
+        <v>37200</v>
+      </c>
+      <c r="V36" s="30" t="s">
+        <v>124</v>
+      </c>
+      <c r="X36" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="AB36" s="28" t="s">
+        <v>182</v>
+      </c>
+      <c r="AC36" s="29"/>
+      <c r="AD36" s="29">
+        <v>37200</v>
+      </c>
+      <c r="AE36" s="30" t="s">
+        <v>124</v>
+      </c>
+      <c r="AK36" s="28" t="s">
+        <v>182</v>
+      </c>
+      <c r="AL36" s="29"/>
+      <c r="AM36" s="29">
+        <v>37200</v>
+      </c>
+      <c r="AN36" s="30" t="s">
+        <v>124</v>
+      </c>
+      <c r="AP36" s="2" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="37" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A37" s="28" t="s">
+        <v>182</v>
+      </c>
+      <c r="B37" s="29"/>
+      <c r="C37" s="29">
+        <v>37200</v>
+      </c>
+      <c r="D37" s="30" t="s">
+        <v>124</v>
+      </c>
+      <c r="J37" s="31" t="s">
+        <v>183</v>
+      </c>
+      <c r="K37" s="32"/>
+      <c r="L37" s="32">
+        <v>20795</v>
+      </c>
+      <c r="M37" s="33" t="s">
+        <v>124</v>
+      </c>
+      <c r="S37" s="31" t="s">
+        <v>183</v>
+      </c>
+      <c r="T37" s="32"/>
+      <c r="U37" s="32">
+        <v>20737</v>
+      </c>
+      <c r="V37" s="33" t="s">
+        <v>124</v>
+      </c>
+      <c r="AB37" s="31" t="s">
+        <v>183</v>
+      </c>
+      <c r="AC37" s="32"/>
+      <c r="AD37" s="32">
+        <v>20737</v>
+      </c>
+      <c r="AE37" s="33" t="s">
+        <v>124</v>
+      </c>
+      <c r="AG37" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="AK37" s="31" t="s">
+        <v>183</v>
+      </c>
+      <c r="AL37" s="32"/>
+      <c r="AM37" s="32">
+        <v>20737</v>
+      </c>
+      <c r="AN37" s="33" t="s">
+        <v>124</v>
+      </c>
+      <c r="AP37" s="2" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="38" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A38" s="31" t="s">
+        <v>183</v>
+      </c>
+      <c r="B38" s="32"/>
+      <c r="C38" s="32">
+        <v>20737</v>
+      </c>
+      <c r="D38" s="33" t="s">
+        <v>124</v>
+      </c>
+      <c r="J38" s="31" t="s">
+        <v>184</v>
+      </c>
+      <c r="K38" s="32"/>
+      <c r="L38" s="32">
+        <v>30140</v>
+      </c>
+      <c r="M38" s="33" t="s">
+        <v>124</v>
+      </c>
+      <c r="O38" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="S38" s="31" t="s">
+        <v>184</v>
+      </c>
+      <c r="T38" s="32"/>
+      <c r="U38" s="32">
+        <v>30140</v>
+      </c>
+      <c r="V38" s="33" t="s">
+        <v>124</v>
+      </c>
+      <c r="X38" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="AB38" s="31" t="s">
+        <v>184</v>
+      </c>
+      <c r="AC38" s="32"/>
+      <c r="AD38" s="32">
+        <v>30140</v>
+      </c>
+      <c r="AE38" s="33" t="s">
+        <v>124</v>
+      </c>
+      <c r="AG38" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="AK38" s="31" t="s">
+        <v>184</v>
+      </c>
+      <c r="AL38" s="32"/>
+      <c r="AM38" s="32">
+        <v>30140</v>
+      </c>
+      <c r="AN38" s="33" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="39" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A39" s="31" t="s">
+        <v>184</v>
+      </c>
+      <c r="B39" s="32"/>
+      <c r="C39" s="32">
+        <v>30140</v>
+      </c>
+      <c r="D39" s="33" t="s">
+        <v>124</v>
+      </c>
+      <c r="J39" s="31" t="s">
+        <v>185</v>
+      </c>
+      <c r="K39" s="32"/>
+      <c r="L39" s="32">
+        <v>9404</v>
+      </c>
+      <c r="M39" s="33" t="s">
+        <v>124</v>
+      </c>
+      <c r="O39" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="S39" s="31" t="s">
+        <v>185</v>
+      </c>
+      <c r="T39" s="32"/>
+      <c r="U39" s="32">
+        <v>9404</v>
+      </c>
+      <c r="V39" s="33" t="s">
+        <v>124</v>
+      </c>
+      <c r="X39" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="AB39" s="31" t="s">
+        <v>185</v>
+      </c>
+      <c r="AC39" s="32"/>
+      <c r="AD39" s="32">
+        <v>9404</v>
+      </c>
+      <c r="AE39" s="33" t="s">
+        <v>124</v>
+      </c>
+      <c r="AG39" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="AK39" s="31" t="s">
+        <v>185</v>
+      </c>
+      <c r="AL39" s="32"/>
+      <c r="AM39" s="32">
+        <v>9404</v>
+      </c>
+      <c r="AN39" s="33" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="40" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A40" s="31" t="s">
+        <v>185</v>
+      </c>
+      <c r="B40" s="32"/>
+      <c r="C40" s="32">
+        <v>9404</v>
+      </c>
+      <c r="D40" s="33" t="s">
+        <v>124</v>
+      </c>
+      <c r="J40" s="31" t="s">
+        <v>186</v>
+      </c>
+      <c r="K40" s="32"/>
+      <c r="L40" s="32">
+        <v>9428</v>
+      </c>
+      <c r="M40" s="33" t="s">
+        <v>124</v>
+      </c>
+      <c r="O40" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="S40" s="31" t="s">
+        <v>186</v>
+      </c>
+      <c r="T40" s="32"/>
+      <c r="U40" s="32">
+        <v>9428</v>
+      </c>
+      <c r="V40" s="33" t="s">
+        <v>124</v>
+      </c>
+      <c r="X40" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="AB40" s="31" t="s">
+        <v>186</v>
+      </c>
+      <c r="AC40" s="32"/>
+      <c r="AD40" s="32">
+        <v>9428</v>
+      </c>
+      <c r="AE40" s="33" t="s">
+        <v>124</v>
+      </c>
+      <c r="AG40" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="AK40" s="31" t="s">
+        <v>186</v>
+      </c>
+      <c r="AL40" s="32"/>
+      <c r="AM40" s="32">
+        <v>9428</v>
+      </c>
+      <c r="AN40" s="33" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="41" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A41" s="31" t="s">
+        <v>186</v>
+      </c>
+      <c r="B41" s="32"/>
+      <c r="C41" s="32">
+        <v>9428</v>
+      </c>
+      <c r="D41" s="33" t="s">
+        <v>124</v>
+      </c>
+      <c r="J41" s="34" t="s">
+        <v>187</v>
+      </c>
+      <c r="K41" s="35"/>
+      <c r="L41" s="35">
+        <v>1600</v>
+      </c>
+      <c r="M41" s="36" t="s">
+        <v>124</v>
+      </c>
+      <c r="S41" s="34" t="s">
+        <v>187</v>
+      </c>
+      <c r="T41" s="35"/>
+      <c r="U41" s="35">
+        <v>1600</v>
+      </c>
+      <c r="V41" s="36" t="s">
+        <v>124</v>
+      </c>
+      <c r="X41" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="AB41" s="34" t="s">
+        <v>187</v>
+      </c>
+      <c r="AC41" s="35"/>
+      <c r="AD41" s="35">
+        <v>1600</v>
+      </c>
+      <c r="AE41" s="36" t="s">
+        <v>124</v>
+      </c>
+      <c r="AK41" s="34" t="s">
+        <v>187</v>
+      </c>
+      <c r="AL41" s="35"/>
+      <c r="AM41" s="35">
+        <v>1600</v>
+      </c>
+      <c r="AN41" s="36" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="42" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A42" s="34" t="s">
+        <v>187</v>
+      </c>
+      <c r="B42" s="35"/>
+      <c r="C42" s="35">
+        <v>1600</v>
+      </c>
+      <c r="D42" s="36" t="s">
+        <v>124</v>
+      </c>
+      <c r="J42" s="28" t="s">
+        <v>172</v>
+      </c>
+      <c r="K42" s="29" t="s">
+        <v>173</v>
+      </c>
+      <c r="L42" s="29" t="s">
+        <v>174</v>
+      </c>
+      <c r="M42" s="30" t="s">
+        <v>175</v>
+      </c>
+      <c r="N42" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="S42" s="28" t="s">
+        <v>172</v>
+      </c>
+      <c r="T42" s="29" t="s">
+        <v>173</v>
+      </c>
+      <c r="U42" s="29" t="s">
+        <v>174</v>
+      </c>
+      <c r="V42" s="30" t="s">
+        <v>175</v>
+      </c>
+      <c r="W42" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="AB42" s="28" t="s">
+        <v>172</v>
+      </c>
+      <c r="AC42" s="29" t="s">
+        <v>173</v>
+      </c>
+      <c r="AD42" s="29" t="s">
+        <v>174</v>
+      </c>
+      <c r="AE42" s="30" t="s">
+        <v>175</v>
+      </c>
+      <c r="AF42" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="AK42" s="28" t="s">
+        <v>172</v>
+      </c>
+      <c r="AL42" s="29" t="s">
+        <v>173</v>
+      </c>
+      <c r="AM42" s="29" t="s">
+        <v>174</v>
+      </c>
+      <c r="AN42" s="30" t="s">
+        <v>175</v>
+      </c>
+      <c r="AO42" s="2" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="43" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A43" s="28" t="s">
+        <v>172</v>
+      </c>
+      <c r="B43" s="29" t="s">
+        <v>173</v>
+      </c>
+      <c r="C43" s="29" t="s">
+        <v>174</v>
+      </c>
+      <c r="D43" s="30" t="s">
+        <v>175</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="J43" s="31" t="s">
+        <v>177</v>
+      </c>
+      <c r="K43" s="32" t="s">
+        <v>178</v>
+      </c>
+      <c r="L43" s="32" t="s">
+        <v>179</v>
+      </c>
+      <c r="M43" s="33" t="s">
+        <v>178</v>
+      </c>
+      <c r="N43" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="S43" s="31" t="s">
+        <v>177</v>
+      </c>
+      <c r="T43" s="32" t="s">
+        <v>178</v>
+      </c>
+      <c r="U43" s="32" t="s">
+        <v>179</v>
+      </c>
+      <c r="V43" s="33" t="s">
+        <v>178</v>
+      </c>
+      <c r="W43" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="AB43" s="31" t="s">
+        <v>177</v>
+      </c>
+      <c r="AC43" s="32" t="s">
+        <v>178</v>
+      </c>
+      <c r="AD43" s="32" t="s">
+        <v>179</v>
+      </c>
+      <c r="AE43" s="33" t="s">
+        <v>178</v>
+      </c>
+      <c r="AF43" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="AK43" s="31" t="s">
+        <v>177</v>
+      </c>
+      <c r="AL43" s="32" t="s">
+        <v>178</v>
+      </c>
+      <c r="AM43" s="32" t="s">
+        <v>179</v>
+      </c>
+      <c r="AN43" s="33" t="s">
+        <v>178</v>
+      </c>
+      <c r="AO43" s="2" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="44" spans="1:43" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="31" t="s">
+        <v>177</v>
+      </c>
+      <c r="B44" s="32" t="s">
+        <v>178</v>
+      </c>
+      <c r="C44" s="32" t="s">
+        <v>179</v>
+      </c>
+      <c r="D44" s="33" t="s">
+        <v>178</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="J44" s="31">
+        <v>0</v>
+      </c>
+      <c r="K44" s="32">
+        <v>9404</v>
+      </c>
+      <c r="L44" s="32">
+        <v>0</v>
+      </c>
+      <c r="M44" s="33">
+        <v>0</v>
+      </c>
+      <c r="O44" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="P44" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="S44" s="31">
+        <v>0</v>
+      </c>
+      <c r="T44" s="32">
+        <v>9404</v>
+      </c>
+      <c r="U44" s="32">
+        <v>0</v>
+      </c>
+      <c r="V44" s="33">
+        <v>0</v>
+      </c>
+      <c r="X44" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="Y44" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="AB44" s="31">
+        <v>0</v>
+      </c>
+      <c r="AC44" s="32">
+        <v>9404</v>
+      </c>
+      <c r="AD44" s="32">
+        <v>0</v>
+      </c>
+      <c r="AE44" s="33">
+        <v>0</v>
+      </c>
+      <c r="AG44" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="AH44" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="AK44" s="31">
+        <v>0</v>
+      </c>
+      <c r="AL44" s="32">
+        <v>9404</v>
+      </c>
+      <c r="AM44" s="32">
+        <v>0</v>
+      </c>
+      <c r="AN44" s="33">
+        <v>0</v>
+      </c>
+      <c r="AP44" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="AQ44" s="2" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="45" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A45" s="31">
+        <v>0</v>
+      </c>
+      <c r="B45" s="32">
+        <v>9404</v>
+      </c>
+      <c r="C45" s="32">
+        <v>0</v>
+      </c>
+      <c r="D45" s="33">
+        <v>0</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="J45" s="31">
+        <v>1353</v>
+      </c>
+      <c r="K45" s="32">
+        <v>9404</v>
+      </c>
+      <c r="L45" s="32">
+        <v>6956</v>
+      </c>
+      <c r="M45" s="33">
+        <v>37200</v>
+      </c>
+      <c r="O45" s="52">
+        <v>-2.0275162925416312E-2</v>
+      </c>
+      <c r="P45" s="2">
+        <v>-28</v>
+      </c>
+      <c r="S45" s="31">
+        <v>1395</v>
+      </c>
+      <c r="T45" s="32">
+        <v>9404</v>
+      </c>
+      <c r="U45" s="32">
+        <v>7059</v>
+      </c>
+      <c r="V45" s="33">
+        <v>37200</v>
+      </c>
+      <c r="X45" s="52">
+        <v>1.0137581462708267E-2</v>
+      </c>
+      <c r="Y45" s="2">
+        <v>14</v>
+      </c>
+      <c r="AB45" s="31">
+        <v>1427</v>
+      </c>
+      <c r="AC45" s="32">
+        <v>9404</v>
+      </c>
+      <c r="AD45" s="32">
+        <v>7099</v>
+      </c>
+      <c r="AE45" s="33">
+        <v>37200</v>
+      </c>
+      <c r="AG45" s="52">
+        <v>3.3309196234612592E-2</v>
+      </c>
+      <c r="AH45" s="2">
+        <v>46</v>
+      </c>
+      <c r="AK45" s="31">
+        <v>1366</v>
+      </c>
+      <c r="AL45" s="32">
+        <v>9404</v>
+      </c>
+      <c r="AM45" s="32">
+        <v>7059</v>
+      </c>
+      <c r="AN45" s="33">
+        <v>37200</v>
+      </c>
+      <c r="AP45" s="52">
+        <v>-1.0861694424330159E-2</v>
+      </c>
+      <c r="AQ45" s="2">
+        <v>-15</v>
+      </c>
+    </row>
+    <row r="46" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A46" s="31">
+        <v>1381</v>
+      </c>
+      <c r="B46" s="32">
+        <v>9404</v>
+      </c>
+      <c r="C46" s="32">
+        <v>7059</v>
+      </c>
+      <c r="D46" s="33">
+        <v>37200</v>
+      </c>
+      <c r="F46" s="52">
+        <f>A46/A27-1</f>
+        <v>0</v>
+      </c>
+      <c r="G46" s="2">
+        <f>A46-A27</f>
+        <v>0</v>
+      </c>
+      <c r="J46" s="31">
+        <v>2039</v>
+      </c>
+      <c r="K46" s="32">
+        <v>6932</v>
+      </c>
+      <c r="L46" s="32">
+        <v>9428</v>
+      </c>
+      <c r="M46" s="33">
+        <v>37200</v>
+      </c>
+      <c r="O46" s="52">
+        <v>0</v>
+      </c>
+      <c r="P46" s="2">
+        <v>0</v>
+      </c>
+      <c r="S46" s="31">
+        <v>2059</v>
+      </c>
+      <c r="T46" s="32">
+        <v>7035</v>
+      </c>
+      <c r="U46" s="32">
+        <v>9428</v>
+      </c>
+      <c r="V46" s="33">
+        <v>37200</v>
+      </c>
+      <c r="X46" s="52">
+        <v>9.8087297694948727E-3</v>
+      </c>
+      <c r="Y46" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB46" s="31">
+        <v>2090</v>
+      </c>
+      <c r="AC46" s="32">
+        <v>7075</v>
+      </c>
+      <c r="AD46" s="32">
+        <v>9428</v>
+      </c>
+      <c r="AE46" s="33">
+        <v>37200</v>
+      </c>
+      <c r="AG46" s="52">
+        <v>2.501226091221187E-2</v>
+      </c>
+      <c r="AH46" s="2">
+        <v>51</v>
+      </c>
+      <c r="AK46" s="31">
+        <v>2018</v>
+      </c>
+      <c r="AL46" s="32">
+        <v>7035</v>
+      </c>
+      <c r="AM46" s="32">
+        <v>9428</v>
+      </c>
+      <c r="AN46" s="33">
+        <v>37200</v>
+      </c>
+      <c r="AP46" s="52">
+        <v>-1.0299166257969561E-2</v>
+      </c>
+      <c r="AQ46" s="2">
+        <v>-21</v>
+      </c>
+    </row>
+    <row r="47" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A47" s="31">
+        <v>2039</v>
+      </c>
+      <c r="B47" s="32">
+        <v>7035</v>
+      </c>
+      <c r="C47" s="32">
+        <v>9428</v>
+      </c>
+      <c r="D47" s="33">
+        <v>37200</v>
+      </c>
+      <c r="F47" s="52">
+        <f t="shared" ref="F47:F48" si="2">A47/A28-1</f>
+        <v>0</v>
+      </c>
+      <c r="G47" s="2">
+        <f t="shared" ref="G47:G48" si="3">A47-A28</f>
+        <v>0</v>
+      </c>
+      <c r="J47" s="31">
+        <v>2357</v>
+      </c>
+      <c r="K47" s="32">
+        <v>0</v>
+      </c>
+      <c r="L47" s="32">
+        <v>9428</v>
+      </c>
+      <c r="M47" s="33">
+        <v>30268</v>
+      </c>
+      <c r="O47" s="52">
+        <v>-2.1168501270110163E-3</v>
+      </c>
+      <c r="P47" s="2">
+        <v>-5</v>
+      </c>
+      <c r="S47" s="31">
+        <v>2379</v>
+      </c>
+      <c r="T47" s="32">
+        <v>0</v>
+      </c>
+      <c r="U47" s="32">
+        <v>9428</v>
+      </c>
+      <c r="V47" s="33">
+        <v>30165</v>
+      </c>
+      <c r="X47" s="52">
+        <v>7.1972904318373665E-3</v>
+      </c>
+      <c r="Y47" s="2">
+        <v>17</v>
+      </c>
+      <c r="AB47" s="31">
+        <v>2424</v>
+      </c>
+      <c r="AC47" s="32">
+        <v>0</v>
+      </c>
+      <c r="AD47" s="32">
+        <v>9428</v>
+      </c>
+      <c r="AE47" s="33">
+        <v>30125</v>
+      </c>
+      <c r="AG47" s="52">
+        <v>2.6248941574936513E-2</v>
+      </c>
+      <c r="AH47" s="2">
+        <v>62</v>
+      </c>
+      <c r="AK47" s="31">
+        <v>2344</v>
+      </c>
+      <c r="AL47" s="32">
+        <v>0</v>
+      </c>
+      <c r="AM47" s="32">
+        <v>9428</v>
+      </c>
+      <c r="AN47" s="33">
+        <v>30165</v>
+      </c>
+      <c r="AP47" s="52">
+        <v>-7.6206604572396364E-3</v>
+      </c>
+      <c r="AQ47" s="2">
+        <v>-18</v>
+      </c>
+    </row>
+    <row r="48" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A48" s="31">
+        <v>2362</v>
+      </c>
+      <c r="B48" s="32">
+        <v>0</v>
+      </c>
+      <c r="C48" s="32">
+        <v>9428</v>
+      </c>
+      <c r="D48" s="33">
+        <v>30165</v>
+      </c>
+      <c r="F48" s="52">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G48" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J48" s="31"/>
+      <c r="K48" s="32"/>
+      <c r="L48" s="32"/>
+      <c r="M48" s="33"/>
+      <c r="S48" s="31"/>
+      <c r="T48" s="32"/>
+      <c r="U48" s="32"/>
+      <c r="V48" s="33"/>
+      <c r="AB48" s="31"/>
+      <c r="AC48" s="32"/>
+      <c r="AD48" s="32"/>
+      <c r="AE48" s="33"/>
+      <c r="AK48" s="31"/>
+      <c r="AL48" s="32"/>
+      <c r="AM48" s="32"/>
+      <c r="AN48" s="33"/>
+    </row>
+    <row r="49" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A49" s="31"/>
+      <c r="B49" s="32"/>
+      <c r="C49" s="32"/>
+      <c r="D49" s="33"/>
+      <c r="J49" s="34"/>
+      <c r="K49" s="35"/>
+      <c r="L49" s="35"/>
+      <c r="M49" s="36"/>
+      <c r="S49" s="34"/>
+      <c r="T49" s="35"/>
+      <c r="U49" s="35"/>
+      <c r="V49" s="36"/>
+      <c r="AB49" s="34"/>
+      <c r="AC49" s="35"/>
+      <c r="AD49" s="35"/>
+      <c r="AE49" s="36"/>
+      <c r="AK49" s="34"/>
+      <c r="AL49" s="35"/>
+      <c r="AM49" s="35"/>
+      <c r="AN49" s="36"/>
+    </row>
+    <row r="50" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A50" s="34"/>
+      <c r="B50" s="35"/>
+      <c r="C50" s="35"/>
+      <c r="D50" s="36"/>
+      <c r="J50" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="O50" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="P50" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="S50" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="X50" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="Y50" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="AB50" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="AG50" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="AH50" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="AK50" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="AP50" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="AQ50" s="2" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="51" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="F51" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="G51" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="J51" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="O51" s="52">
+        <v>9.7014925373133387E-3</v>
+      </c>
+      <c r="P51" s="2">
+        <v>13</v>
+      </c>
+      <c r="S51" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="X51" s="52">
+        <v>4.1044776119403048E-2</v>
+      </c>
+      <c r="Y51" s="2">
+        <v>55</v>
+      </c>
+      <c r="AB51" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="AG51" s="52">
+        <v>6.4925373134328446E-2</v>
+      </c>
+      <c r="AH51" s="2">
+        <v>87</v>
+      </c>
+      <c r="AK51" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="AP51" s="52">
+        <v>1.9402985074626899E-2</v>
+      </c>
+      <c r="AQ51" s="2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="52" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="F52" s="52">
+        <f>A46/A12-1</f>
+        <v>3.0597014925373145E-2</v>
+      </c>
+      <c r="G52" s="2">
+        <f>A46-A12</f>
+        <v>41</v>
+      </c>
+      <c r="O52" s="52">
+        <v>9.4059405940594143E-3</v>
+      </c>
+      <c r="P52" s="2">
+        <v>19</v>
+      </c>
+      <c r="X52" s="52">
+        <v>1.9306930693069324E-2</v>
+      </c>
+      <c r="Y52" s="2">
+        <v>39</v>
+      </c>
+      <c r="AG52" s="52">
+        <v>3.4653465346534684E-2</v>
+      </c>
+      <c r="AH52" s="2">
+        <v>70</v>
+      </c>
+      <c r="AP52" s="52">
+        <v>-9.9009900990099098E-4</v>
+      </c>
+      <c r="AQ52" s="2">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="F53" s="52">
+        <f t="shared" ref="F53:F54" si="4">A47/A13-1</f>
+        <v>9.4059405940594143E-3</v>
+      </c>
+      <c r="G53" s="2">
+        <f t="shared" ref="G53:G54" si="5">A47-A13</f>
+        <v>19</v>
+      </c>
+      <c r="O53" s="52">
+        <v>1.5948275862069039E-2</v>
+      </c>
+      <c r="P53" s="2">
+        <v>37</v>
+      </c>
+      <c r="X53" s="52">
+        <v>2.543103448275863E-2</v>
+      </c>
+      <c r="Y53" s="2">
+        <v>59</v>
+      </c>
+      <c r="AG53" s="52">
+        <v>4.482758620689653E-2</v>
+      </c>
+      <c r="AH53" s="2">
+        <v>104</v>
+      </c>
+      <c r="AP53" s="52">
+        <v>1.0344827586206806E-2</v>
+      </c>
+      <c r="AQ53" s="2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="54" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="F54" s="52">
+        <f t="shared" si="4"/>
+        <v>1.8103448275861966E-2</v>
+      </c>
+      <c r="G54" s="2">
+        <f t="shared" si="5"/>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="8">
+    <mergeCell ref="U35:V35"/>
+    <mergeCell ref="AD35:AE35"/>
+    <mergeCell ref="AM35:AN35"/>
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="L35:M35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -10935,6 +12360,70 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:G11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>0.98</v>
+      </c>
+      <c r="E7">
+        <f>21/23</f>
+        <v>0.91304347826086951</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>1.65</v>
+      </c>
+      <c r="G9">
+        <f>0.702/0.68</f>
+        <v>1.0323529411764705</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <f>PRODUCT(B3:B9)</f>
+        <v>21.023288054999998</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AR61"/>
   <sheetViews>
@@ -16141,11 +17630,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N41"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
@@ -16895,7 +18384,7 @@
         <v>0.99</v>
       </c>
       <c r="J30" s="32" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="K30" s="32">
         <f>B15*C15/K29</f>

</xml_diff>